<commit_message>
Indsat data fra kladder i VT AGR&IND
Kopieret data over fra de kladder, jeg har lavet i den seperate mappe til de rigtige VT-filer og omdøbt VT-filerne, så det ligner, jeg sletter to filer og laver to nye. Jeg retter også lidt i strukturen af VT-filerne, hvilket sikkert resulterer i, at EB skal kigge efter nye tags. Den tid den sorg
</commit_message>
<xml_diff>
--- a/AGR & IND - Jonathans kladder/nrg_bal_2010_agr&ind.xlsx
+++ b/AGR & IND - Jonathans kladder/nrg_bal_2010_agr&ind.xlsx
@@ -321,8 +321,8 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="2">
-    <numFmt numFmtId="165" formatCode="#,##0.000"/>
-    <numFmt numFmtId="167" formatCode="0.0"/>
+    <numFmt numFmtId="164" formatCode="#,##0.000"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
   </numFmts>
   <fonts count="12" x14ac:knownFonts="1">
     <font>
@@ -522,7 +522,7 @@
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="165" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="164" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -531,21 +531,14 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="167" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="167" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center" shrinkToFit="1"/>
     </xf>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="7" fillId="6" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" indent="1"/>
     </xf>
@@ -557,6 +550,13 @@
     </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="2" applyFont="1"/>
     <xf numFmtId="0" fontId="11" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -933,22 +933,22 @@
       <c r="A8" s="9" t="s">
         <v>3</v>
       </c>
-      <c r="B8" s="18" t="s">
+      <c r="B8" s="27" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="19"/>
-      <c r="D8" s="19"/>
-      <c r="E8" s="19"/>
-      <c r="F8" s="19"/>
-      <c r="G8" s="19"/>
-      <c r="H8" s="19"/>
-      <c r="I8" s="19"/>
-      <c r="J8" s="19"/>
-      <c r="K8" s="19"/>
-      <c r="L8" s="19"/>
-      <c r="M8" s="19"/>
-      <c r="N8" s="19"/>
-      <c r="O8" s="19"/>
+      <c r="C8" s="28"/>
+      <c r="D8" s="28"/>
+      <c r="E8" s="28"/>
+      <c r="F8" s="28"/>
+      <c r="G8" s="28"/>
+      <c r="H8" s="28"/>
+      <c r="I8" s="28"/>
+      <c r="J8" s="28"/>
+      <c r="K8" s="28"/>
+      <c r="L8" s="28"/>
+      <c r="M8" s="28"/>
+      <c r="N8" s="28"/>
+      <c r="O8" s="28"/>
     </row>
     <row r="10" spans="1:15" x14ac:dyDescent="0.3">
       <c r="A10" s="2" t="s">
@@ -1357,9 +1357,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AK45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A6" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <pane xSplit="2" topLeftCell="R1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="C6" sqref="C6:U6"/>
+      <selection pane="topRight" activeCell="R29" sqref="R29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="11.4" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -1403,22 +1403,22 @@
     <col min="37" max="37" width="5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:37" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A1" s="3" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="2" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:37" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="3" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:37" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A3" s="2" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="5" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:37" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>12</v>
       </c>
@@ -1426,185 +1426,185 @@
         <v>15</v>
       </c>
     </row>
-    <row r="6" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:37" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>16</v>
       </c>
-      <c r="C6" s="28" t="s">
+      <c r="C6" s="25" t="s">
         <v>91</v>
       </c>
-      <c r="D6" s="28" t="s">
+      <c r="D6" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="28" t="s">
+      <c r="E6" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="F6" s="28" t="s">
+      <c r="F6" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="G6" s="28" t="s">
+      <c r="G6" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="H6" s="28" t="s">
+      <c r="H6" s="25" t="s">
         <v>92</v>
       </c>
-      <c r="I6" s="28" t="s">
+      <c r="I6" s="25" t="s">
         <v>93</v>
       </c>
-      <c r="J6" s="28" t="s">
+      <c r="J6" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="K6" s="28" t="s">
+      <c r="K6" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="L6" s="28" t="s">
+      <c r="L6" s="25" t="s">
         <v>94</v>
       </c>
-      <c r="M6" s="28" t="s">
+      <c r="M6" s="25" t="s">
         <v>95</v>
       </c>
-      <c r="N6" s="28" t="s">
+      <c r="N6" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="O6" s="28" t="s">
+      <c r="O6" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="P6" s="28" t="s">
+      <c r="P6" s="25" t="s">
         <v>40</v>
       </c>
-      <c r="Q6" s="29" t="s">
+      <c r="Q6" s="26" t="s">
         <v>96</v>
       </c>
-      <c r="R6" s="28" t="s">
+      <c r="R6" s="25" t="s">
         <v>97</v>
       </c>
-      <c r="S6" s="28" t="s">
+      <c r="S6" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="T6" s="28" t="s">
+      <c r="T6" s="25" t="s">
         <v>98</v>
       </c>
-      <c r="U6" s="28" t="s">
+      <c r="U6" s="25" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="8" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:37" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A8" s="16" t="s">
         <v>64</v>
       </c>
-      <c r="B8" s="20" t="s">
+      <c r="B8" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="C8" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="D8" s="20" t="s">
+      <c r="C8" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="D8" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="E8" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="F8" s="20" t="s">
+      <c r="E8" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="F8" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="G8" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="H8" s="20" t="s">
+      <c r="G8" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="H8" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="I8" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="J8" s="20" t="s">
+      <c r="I8" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="J8" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="K8" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="L8" s="20" t="s">
+      <c r="K8" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="L8" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="M8" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="N8" s="20" t="s">
+      <c r="M8" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="N8" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="O8" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="P8" s="20" t="s">
+      <c r="O8" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="P8" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="Q8" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="R8" s="20" t="s">
+      <c r="Q8" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="R8" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="S8" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="T8" s="20" t="s">
+      <c r="S8" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="T8" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="U8" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="V8" s="20" t="s">
+      <c r="U8" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="V8" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="W8" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="X8" s="20" t="s">
+      <c r="W8" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="X8" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="Y8" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="Z8" s="20" t="s">
+      <c r="Y8" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="Z8" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="AA8" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="AB8" s="20" t="s">
+      <c r="AA8" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="AB8" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="AC8" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="AD8" s="20" t="s">
+      <c r="AC8" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="AD8" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="AE8" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="AF8" s="20" t="s">
+      <c r="AE8" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="AF8" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="AG8" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="AH8" s="20" t="s">
+      <c r="AG8" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="AH8" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="AI8" s="20" t="s">
-        <v>65</v>
-      </c>
-      <c r="AJ8" s="20" t="s">
+      <c r="AI8" s="29" t="s">
+        <v>65</v>
+      </c>
+      <c r="AJ8" s="29" t="s">
         <v>60</v>
       </c>
-      <c r="AK8" s="20" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="9" spans="1:37" x14ac:dyDescent="0.3">
+      <c r="AK8" s="29" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="9" spans="1:37" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A9" s="16" t="s">
         <v>66</v>
       </c>
@@ -1657,10 +1657,10 @@
         <v>88</v>
       </c>
       <c r="R9" s="17" t="s">
+        <v>56</v>
+      </c>
+      <c r="S9" s="17" t="s">
         <v>55</v>
-      </c>
-      <c r="S9" s="17" t="s">
-        <v>56</v>
       </c>
       <c r="T9" s="17" t="s">
         <v>89</v>
@@ -1675,7 +1675,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="10" spans="1:37" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:37" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A10" s="4" t="s">
         <v>67</v>
       </c>
@@ -1746,73 +1746,73 @@
         <v>65</v>
       </c>
     </row>
-    <row r="11" spans="1:37" x14ac:dyDescent="0.3">
-      <c r="A11" s="25" t="s">
+    <row r="11" spans="1:37" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A11" s="22" t="s">
         <v>72</v>
       </c>
-      <c r="B11" s="22">
+      <c r="B11" s="19">
         <v>2372614.094</v>
       </c>
-      <c r="C11" s="23">
+      <c r="C11" s="20">
         <v>137677.60399999999</v>
       </c>
-      <c r="D11" s="22">
-        <v>0</v>
-      </c>
-      <c r="E11" s="22" t="s">
+      <c r="D11" s="19">
+        <v>0</v>
+      </c>
+      <c r="E11" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="F11" s="22">
+      <c r="F11" s="19">
         <v>168128.35399999999</v>
       </c>
-      <c r="G11" s="22">
+      <c r="G11" s="19">
         <v>15620.864</v>
       </c>
-      <c r="H11" s="22">
+      <c r="H11" s="19">
         <v>10955.378000000001</v>
       </c>
-      <c r="I11" s="22">
-        <v>0</v>
-      </c>
-      <c r="J11" s="22">
-        <v>0</v>
-      </c>
-      <c r="K11" s="22">
-        <v>0</v>
-      </c>
-      <c r="L11" s="22">
+      <c r="I11" s="19">
+        <v>0</v>
+      </c>
+      <c r="J11" s="19">
+        <v>0</v>
+      </c>
+      <c r="K11" s="19">
+        <v>0</v>
+      </c>
+      <c r="L11" s="19">
         <v>72878.604999999996</v>
       </c>
-      <c r="M11" s="22">
+      <c r="M11" s="19">
         <v>59432.603999999999</v>
       </c>
-      <c r="N11" s="22">
-        <v>0</v>
-      </c>
-      <c r="O11" s="22">
+      <c r="N11" s="19">
+        <v>0</v>
+      </c>
+      <c r="O11" s="19">
         <f>F11-SUM(G11:N11)</f>
         <v>9240.9029999999912</v>
       </c>
-      <c r="P11" s="22">
+      <c r="P11" s="19">
         <v>843797.61600000004</v>
       </c>
-      <c r="Q11" s="24">
+      <c r="Q11" s="21">
         <v>152304.52000000002</v>
       </c>
-      <c r="R11" s="22">
+      <c r="R11" s="19">
+        <v>146022</v>
+      </c>
+      <c r="S11" s="19">
         <v>822618</v>
       </c>
-      <c r="S11" s="22">
-        <v>146022</v>
-      </c>
-      <c r="T11" s="23">
+      <c r="T11" s="20">
         <v>102066</v>
       </c>
-      <c r="U11" s="22">
+      <c r="U11" s="19">
         <f>SUM(G11:T11)+C11</f>
         <v>2372614.094</v>
       </c>
-      <c r="V11" s="22">
+      <c r="V11" s="19">
         <f>U11-B11</f>
         <v>0</v>
       </c>
@@ -1820,73 +1820,73 @@
         <v>65</v>
       </c>
     </row>
-    <row r="12" spans="1:37" x14ac:dyDescent="0.3">
-      <c r="A12" s="26" t="s">
+    <row r="12" spans="1:37" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A12" s="23" t="s">
         <v>73</v>
       </c>
-      <c r="B12" s="23">
+      <c r="B12" s="20">
         <v>330774.06900000002</v>
       </c>
-      <c r="C12" s="22">
+      <c r="C12" s="19">
         <v>29540.659</v>
       </c>
-      <c r="D12" s="23">
-        <v>0</v>
-      </c>
-      <c r="E12" s="23" t="s">
+      <c r="D12" s="20">
+        <v>0</v>
+      </c>
+      <c r="E12" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="F12" s="23">
+      <c r="F12" s="20">
         <v>4206.5839999999998</v>
       </c>
-      <c r="G12" s="23">
-        <v>0</v>
-      </c>
-      <c r="H12" s="23">
+      <c r="G12" s="20">
+        <v>0</v>
+      </c>
+      <c r="H12" s="20">
         <v>2623.7669999999998</v>
       </c>
-      <c r="I12" s="23">
-        <v>0</v>
-      </c>
-      <c r="J12" s="23">
-        <v>0</v>
-      </c>
-      <c r="K12" s="23">
-        <v>0</v>
-      </c>
-      <c r="L12" s="23">
+      <c r="I12" s="20">
+        <v>0</v>
+      </c>
+      <c r="J12" s="20">
+        <v>0</v>
+      </c>
+      <c r="K12" s="20">
+        <v>0</v>
+      </c>
+      <c r="L12" s="20">
         <v>1286.8499999999999</v>
       </c>
-      <c r="M12" s="23">
+      <c r="M12" s="20">
         <v>201.74</v>
       </c>
-      <c r="N12" s="23">
-        <v>0</v>
-      </c>
-      <c r="O12" s="22">
+      <c r="N12" s="20">
+        <v>0</v>
+      </c>
+      <c r="O12" s="19">
         <f t="shared" ref="O12:O26" si="0">F12-SUM(G12:N12)</f>
         <v>94.226999999999862</v>
       </c>
-      <c r="P12" s="23">
+      <c r="P12" s="20">
         <v>99519.558000000005</v>
       </c>
-      <c r="Q12" s="24">
+      <c r="Q12" s="21">
         <v>134.768</v>
       </c>
-      <c r="R12" s="23">
+      <c r="R12" s="20">
+        <v>1774</v>
+      </c>
+      <c r="S12" s="20">
         <v>97534.8</v>
       </c>
-      <c r="S12" s="23">
-        <v>1774</v>
-      </c>
-      <c r="T12" s="22">
+      <c r="T12" s="19">
         <v>98063.7</v>
       </c>
-      <c r="U12" s="22">
+      <c r="U12" s="19">
         <f t="shared" ref="U12:U26" si="1">SUM(G12:T12)+C12</f>
         <v>330774.06900000002</v>
       </c>
-      <c r="V12" s="22">
+      <c r="V12" s="19">
         <f t="shared" ref="V12:V26" si="2">U12-B12</f>
         <v>0</v>
       </c>
@@ -1894,73 +1894,73 @@
         <v>65</v>
       </c>
     </row>
-    <row r="13" spans="1:37" x14ac:dyDescent="0.3">
-      <c r="A13" s="26" t="s">
+    <row r="13" spans="1:37" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A13" s="23" t="s">
         <v>74</v>
       </c>
-      <c r="B13" s="22">
+      <c r="B13" s="19">
         <v>588419.799</v>
       </c>
-      <c r="C13" s="23">
+      <c r="C13" s="20">
         <v>21580.32</v>
       </c>
-      <c r="D13" s="22">
-        <v>0</v>
-      </c>
-      <c r="E13" s="22" t="s">
+      <c r="D13" s="19">
+        <v>0</v>
+      </c>
+      <c r="E13" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="F13" s="22">
+      <c r="F13" s="19">
         <v>62032.112000000001</v>
       </c>
-      <c r="G13" s="22">
+      <c r="G13" s="19">
         <v>13158.88</v>
       </c>
-      <c r="H13" s="22">
-        <v>0</v>
-      </c>
-      <c r="I13" s="22">
-        <v>0</v>
-      </c>
-      <c r="J13" s="22">
-        <v>0</v>
-      </c>
-      <c r="K13" s="22">
-        <v>0</v>
-      </c>
-      <c r="L13" s="22">
+      <c r="H13" s="19">
+        <v>0</v>
+      </c>
+      <c r="I13" s="19">
+        <v>0</v>
+      </c>
+      <c r="J13" s="19">
+        <v>0</v>
+      </c>
+      <c r="K13" s="19">
+        <v>0</v>
+      </c>
+      <c r="L13" s="19">
         <v>2916.86</v>
       </c>
-      <c r="M13" s="22">
+      <c r="M13" s="19">
         <v>45956.372000000003</v>
       </c>
-      <c r="N13" s="22">
-        <v>0</v>
-      </c>
-      <c r="O13" s="22">
+      <c r="N13" s="19">
+        <v>0</v>
+      </c>
+      <c r="O13" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="P13" s="22">
+      <c r="P13" s="19">
         <v>224126.00700000001</v>
       </c>
-      <c r="Q13" s="24">
+      <c r="Q13" s="21">
         <v>13253.46</v>
       </c>
-      <c r="R13" s="22">
+      <c r="R13" s="19">
+        <v>75475</v>
+      </c>
+      <c r="S13" s="19">
         <v>188413.2</v>
       </c>
-      <c r="S13" s="22">
-        <v>75475</v>
-      </c>
-      <c r="T13" s="23">
+      <c r="T13" s="20">
         <v>3539.7</v>
       </c>
-      <c r="U13" s="22">
+      <c r="U13" s="19">
         <f t="shared" si="1"/>
         <v>588419.799</v>
       </c>
-      <c r="V13" s="22">
+      <c r="V13" s="19">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -1968,73 +1968,73 @@
         <v>65</v>
       </c>
     </row>
-    <row r="14" spans="1:37" x14ac:dyDescent="0.3">
-      <c r="A14" s="26" t="s">
+    <row r="14" spans="1:37" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A14" s="23" t="s">
         <v>75</v>
       </c>
-      <c r="B14" s="23">
+      <c r="B14" s="20">
         <v>89446.138000000006</v>
       </c>
-      <c r="C14" s="22">
+      <c r="C14" s="19">
         <v>1043.671</v>
       </c>
-      <c r="D14" s="23">
-        <v>0</v>
-      </c>
-      <c r="E14" s="23" t="s">
+      <c r="D14" s="20">
+        <v>0</v>
+      </c>
+      <c r="E14" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="F14" s="23">
+      <c r="F14" s="20">
         <v>4189.7929999999997</v>
       </c>
-      <c r="G14" s="23">
-        <v>0</v>
-      </c>
-      <c r="H14" s="23">
+      <c r="G14" s="20">
+        <v>0</v>
+      </c>
+      <c r="H14" s="20">
         <v>184.124</v>
       </c>
-      <c r="I14" s="23">
-        <v>0</v>
-      </c>
-      <c r="J14" s="23">
-        <v>0</v>
-      </c>
-      <c r="K14" s="23">
-        <v>0</v>
-      </c>
-      <c r="L14" s="23">
+      <c r="I14" s="20">
+        <v>0</v>
+      </c>
+      <c r="J14" s="20">
+        <v>0</v>
+      </c>
+      <c r="K14" s="20">
+        <v>0</v>
+      </c>
+      <c r="L14" s="20">
         <v>1372.64</v>
       </c>
-      <c r="M14" s="23">
+      <c r="M14" s="20">
         <v>968.35199999999998</v>
       </c>
-      <c r="N14" s="23">
-        <v>0</v>
-      </c>
-      <c r="O14" s="22">
+      <c r="N14" s="20">
+        <v>0</v>
+      </c>
+      <c r="O14" s="19">
         <f t="shared" si="0"/>
         <v>1664.6769999999997</v>
       </c>
-      <c r="P14" s="23">
+      <c r="P14" s="20">
         <v>32190.673999999999</v>
       </c>
-      <c r="Q14" s="24">
+      <c r="Q14" s="21">
         <v>329</v>
       </c>
-      <c r="R14" s="23">
+      <c r="R14" s="20">
+        <v>2571</v>
+      </c>
+      <c r="S14" s="20">
         <v>49122</v>
       </c>
-      <c r="S14" s="23">
-        <v>2571</v>
-      </c>
-      <c r="T14" s="22">
-        <v>0</v>
-      </c>
-      <c r="U14" s="22">
+      <c r="T14" s="19">
+        <v>0</v>
+      </c>
+      <c r="U14" s="19">
         <f t="shared" si="1"/>
         <v>89446.138000000006</v>
       </c>
-      <c r="V14" s="22">
+      <c r="V14" s="19">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -2042,73 +2042,73 @@
         <v>65</v>
       </c>
     </row>
-    <row r="15" spans="1:37" x14ac:dyDescent="0.3">
-      <c r="A15" s="26" t="s">
+    <row r="15" spans="1:37" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A15" s="23" t="s">
         <v>76</v>
       </c>
-      <c r="B15" s="22">
+      <c r="B15" s="19">
         <v>272879.16200000001</v>
       </c>
-      <c r="C15" s="23">
+      <c r="C15" s="20">
         <v>56552.896000000001</v>
       </c>
-      <c r="D15" s="22">
-        <v>0</v>
-      </c>
-      <c r="E15" s="22" t="s">
+      <c r="D15" s="19">
+        <v>0</v>
+      </c>
+      <c r="E15" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="F15" s="22">
+      <c r="F15" s="19">
         <v>28630.937999999998</v>
       </c>
-      <c r="G15" s="22">
-        <v>0</v>
-      </c>
-      <c r="H15" s="22">
+      <c r="G15" s="19">
+        <v>0</v>
+      </c>
+      <c r="H15" s="19">
         <v>1242.837</v>
       </c>
-      <c r="I15" s="22">
-        <v>0</v>
-      </c>
-      <c r="J15" s="22">
-        <v>0</v>
-      </c>
-      <c r="K15" s="22">
-        <v>0</v>
-      </c>
-      <c r="L15" s="22">
+      <c r="I15" s="19">
+        <v>0</v>
+      </c>
+      <c r="J15" s="19">
+        <v>0</v>
+      </c>
+      <c r="K15" s="19">
+        <v>0</v>
+      </c>
+      <c r="L15" s="19">
         <v>12396.655000000001</v>
       </c>
-      <c r="M15" s="22">
+      <c r="M15" s="19">
         <v>7746.8159999999998</v>
       </c>
-      <c r="N15" s="22">
-        <v>0</v>
-      </c>
-      <c r="O15" s="22">
+      <c r="N15" s="19">
+        <v>0</v>
+      </c>
+      <c r="O15" s="19">
         <f t="shared" si="0"/>
         <v>7244.6299999999974</v>
       </c>
-      <c r="P15" s="22">
+      <c r="P15" s="19">
         <v>102503.992</v>
       </c>
-      <c r="Q15" s="24">
+      <c r="Q15" s="21">
         <v>40433.835999999996</v>
       </c>
-      <c r="R15" s="22">
+      <c r="R15" s="19">
+        <v>608</v>
+      </c>
+      <c r="S15" s="19">
         <v>44042.400000000001</v>
       </c>
-      <c r="S15" s="22">
-        <v>608</v>
-      </c>
-      <c r="T15" s="23">
+      <c r="T15" s="20">
         <v>107.1</v>
       </c>
-      <c r="U15" s="22">
+      <c r="U15" s="19">
         <f t="shared" si="1"/>
         <v>272879.16200000001</v>
       </c>
-      <c r="V15" s="22">
+      <c r="V15" s="19">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -2116,73 +2116,73 @@
         <v>65</v>
       </c>
     </row>
-    <row r="16" spans="1:37" x14ac:dyDescent="0.3">
-      <c r="A16" s="26" t="s">
+    <row r="16" spans="1:37" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A16" s="23" t="s">
         <v>77</v>
       </c>
-      <c r="B16" s="23">
+      <c r="B16" s="20">
         <v>123559.23299999999</v>
       </c>
-      <c r="C16" s="22">
+      <c r="C16" s="19">
         <v>687.6</v>
       </c>
-      <c r="D16" s="23">
-        <v>0</v>
-      </c>
-      <c r="E16" s="23" t="s">
+      <c r="D16" s="20">
+        <v>0</v>
+      </c>
+      <c r="E16" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="F16" s="23">
+      <c r="F16" s="20">
         <v>4004.915</v>
       </c>
-      <c r="G16" s="23">
-        <v>0</v>
-      </c>
-      <c r="H16" s="23">
+      <c r="G16" s="20">
+        <v>0</v>
+      </c>
+      <c r="H16" s="20">
         <v>230.155</v>
       </c>
-      <c r="I16" s="23">
-        <v>0</v>
-      </c>
-      <c r="J16" s="23">
-        <v>0</v>
-      </c>
-      <c r="K16" s="23">
-        <v>0</v>
-      </c>
-      <c r="L16" s="23">
+      <c r="I16" s="20">
+        <v>0</v>
+      </c>
+      <c r="J16" s="20">
+        <v>0</v>
+      </c>
+      <c r="K16" s="20">
+        <v>0</v>
+      </c>
+      <c r="L16" s="20">
         <v>3774.76</v>
       </c>
-      <c r="M16" s="23">
-        <v>0</v>
-      </c>
-      <c r="N16" s="23">
-        <v>0</v>
-      </c>
-      <c r="O16" s="22">
+      <c r="M16" s="20">
+        <v>0</v>
+      </c>
+      <c r="N16" s="20">
+        <v>0</v>
+      </c>
+      <c r="O16" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="P16" s="23">
+      <c r="P16" s="20">
         <v>38022.741999999998</v>
       </c>
-      <c r="Q16" s="24">
+      <c r="Q16" s="21">
         <v>340.07600000000002</v>
       </c>
-      <c r="R16" s="23">
+      <c r="R16" s="20">
+        <v>15937</v>
+      </c>
+      <c r="S16" s="20">
         <v>64216.800000000003</v>
       </c>
-      <c r="S16" s="23">
-        <v>15937</v>
-      </c>
-      <c r="T16" s="22">
+      <c r="T16" s="19">
         <v>350.1</v>
       </c>
-      <c r="U16" s="22">
+      <c r="U16" s="19">
         <f t="shared" si="1"/>
         <v>123559.23300000001</v>
       </c>
-      <c r="V16" s="22">
+      <c r="V16" s="19">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -2190,73 +2190,73 @@
         <v>65</v>
       </c>
     </row>
-    <row r="17" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A17" s="26" t="s">
+    <row r="17" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A17" s="23" t="s">
         <v>78</v>
       </c>
-      <c r="B17" s="22">
+      <c r="B17" s="19">
         <v>232432.842</v>
       </c>
-      <c r="C17" s="23">
+      <c r="C17" s="20">
         <v>720.02099999999996</v>
       </c>
-      <c r="D17" s="22">
-        <v>0</v>
-      </c>
-      <c r="E17" s="22" t="s">
+      <c r="D17" s="19">
+        <v>0</v>
+      </c>
+      <c r="E17" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="F17" s="22">
+      <c r="F17" s="19">
         <v>23341.79</v>
       </c>
-      <c r="G17" s="22">
-        <v>0</v>
-      </c>
-      <c r="H17" s="22">
+      <c r="G17" s="19">
+        <v>0</v>
+      </c>
+      <c r="H17" s="19">
         <v>2439.643</v>
       </c>
-      <c r="I17" s="22">
-        <v>0</v>
-      </c>
-      <c r="J17" s="22">
-        <v>0</v>
-      </c>
-      <c r="K17" s="22">
-        <v>0</v>
-      </c>
-      <c r="L17" s="22">
+      <c r="I17" s="19">
+        <v>0</v>
+      </c>
+      <c r="J17" s="19">
+        <v>0</v>
+      </c>
+      <c r="K17" s="19">
+        <v>0</v>
+      </c>
+      <c r="L17" s="19">
         <v>20718.285</v>
       </c>
-      <c r="M17" s="22">
+      <c r="M17" s="19">
         <v>121.044</v>
       </c>
-      <c r="N17" s="22">
-        <v>0</v>
-      </c>
-      <c r="O17" s="22">
+      <c r="N17" s="19">
+        <v>0</v>
+      </c>
+      <c r="O17" s="19">
         <f t="shared" si="0"/>
         <v>62.817999999999302</v>
       </c>
-      <c r="P17" s="22">
+      <c r="P17" s="19">
         <v>74901.570999999996</v>
       </c>
-      <c r="Q17" s="24">
+      <c r="Q17" s="21">
         <v>1857.46</v>
       </c>
-      <c r="R17" s="22">
+      <c r="R17" s="19">
+        <v>13136</v>
+      </c>
+      <c r="S17" s="19">
         <v>118476</v>
       </c>
-      <c r="S17" s="22">
-        <v>13136</v>
-      </c>
-      <c r="T17" s="23">
-        <v>0</v>
-      </c>
-      <c r="U17" s="22">
+      <c r="T17" s="20">
+        <v>0</v>
+      </c>
+      <c r="U17" s="19">
         <f t="shared" si="1"/>
         <v>232432.842</v>
       </c>
-      <c r="V17" s="22">
+      <c r="V17" s="19">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -2264,73 +2264,73 @@
         <v>65</v>
       </c>
     </row>
-    <row r="18" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A18" s="27" t="s">
+    <row r="18" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A18" s="24" t="s">
         <v>79</v>
       </c>
-      <c r="B18" s="23">
+      <c r="B18" s="20">
         <v>18503.191999999999</v>
       </c>
-      <c r="C18" s="22">
+      <c r="C18" s="19">
         <v>2252.96</v>
       </c>
-      <c r="D18" s="23">
-        <v>0</v>
-      </c>
-      <c r="E18" s="23" t="s">
+      <c r="D18" s="20">
+        <v>0</v>
+      </c>
+      <c r="E18" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="F18" s="23">
+      <c r="F18" s="20">
         <v>1661.577</v>
       </c>
-      <c r="G18" s="23">
-        <v>0</v>
-      </c>
-      <c r="H18" s="23">
+      <c r="G18" s="20">
+        <v>0</v>
+      </c>
+      <c r="H18" s="20">
         <v>414.279</v>
       </c>
-      <c r="I18" s="23">
-        <v>0</v>
-      </c>
-      <c r="J18" s="23">
-        <v>0</v>
-      </c>
-      <c r="K18" s="23">
-        <v>0</v>
-      </c>
-      <c r="L18" s="23">
+      <c r="I18" s="20">
+        <v>0</v>
+      </c>
+      <c r="J18" s="20">
+        <v>0</v>
+      </c>
+      <c r="K18" s="20">
+        <v>0</v>
+      </c>
+      <c r="L18" s="20">
         <v>1072.375</v>
       </c>
-      <c r="M18" s="23">
+      <c r="M18" s="20">
         <v>80.695999999999998</v>
       </c>
-      <c r="N18" s="23">
-        <v>0</v>
-      </c>
-      <c r="O18" s="22">
+      <c r="N18" s="20">
+        <v>0</v>
+      </c>
+      <c r="O18" s="19">
         <f t="shared" si="0"/>
         <v>94.227000000000089</v>
       </c>
-      <c r="P18" s="23">
+      <c r="P18" s="20">
         <v>6125.4709999999995</v>
       </c>
-      <c r="Q18" s="24">
+      <c r="Q18" s="21">
         <v>638.38400000000001</v>
       </c>
-      <c r="R18" s="23">
+      <c r="R18" s="20">
+        <v>56</v>
+      </c>
+      <c r="S18" s="20">
         <v>7768.8</v>
       </c>
-      <c r="S18" s="23">
-        <v>56</v>
-      </c>
-      <c r="T18" s="22">
-        <v>0</v>
-      </c>
-      <c r="U18" s="22">
+      <c r="T18" s="19">
+        <v>0</v>
+      </c>
+      <c r="U18" s="19">
         <f t="shared" si="1"/>
         <v>18503.191999999999</v>
       </c>
-      <c r="V18" s="22">
+      <c r="V18" s="19">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -2338,73 +2338,73 @@
         <v>65</v>
       </c>
     </row>
-    <row r="19" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A19" s="27" t="s">
+    <row r="19" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A19" s="24" t="s">
         <v>80</v>
       </c>
-      <c r="B19" s="22">
+      <c r="B19" s="19">
         <v>201710.19500000001</v>
       </c>
-      <c r="C19" s="23">
+      <c r="C19" s="20">
         <v>8542.4750000000004</v>
       </c>
-      <c r="D19" s="22">
-        <v>0</v>
-      </c>
-      <c r="E19" s="22" t="s">
+      <c r="D19" s="19">
+        <v>0</v>
+      </c>
+      <c r="E19" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="F19" s="22">
+      <c r="F19" s="19">
         <v>16688.75</v>
       </c>
-      <c r="G19" s="22">
-        <v>0</v>
-      </c>
-      <c r="H19" s="22">
+      <c r="G19" s="19">
+        <v>0</v>
+      </c>
+      <c r="H19" s="19">
         <v>1795.2090000000001</v>
       </c>
-      <c r="I19" s="22">
-        <v>0</v>
-      </c>
-      <c r="J19" s="22">
-        <v>0</v>
-      </c>
-      <c r="K19" s="22">
-        <v>0</v>
-      </c>
-      <c r="L19" s="22">
+      <c r="I19" s="19">
+        <v>0</v>
+      </c>
+      <c r="J19" s="19">
+        <v>0</v>
+      </c>
+      <c r="K19" s="19">
+        <v>0</v>
+      </c>
+      <c r="L19" s="19">
         <v>12997.184999999999</v>
       </c>
-      <c r="M19" s="22">
+      <c r="M19" s="19">
         <v>1896.356</v>
       </c>
-      <c r="N19" s="22">
-        <v>0</v>
-      </c>
-      <c r="O19" s="22">
+      <c r="N19" s="19">
+        <v>0</v>
+      </c>
+      <c r="O19" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="P19" s="22">
+      <c r="P19" s="19">
         <v>105401.126</v>
       </c>
-      <c r="Q19" s="24">
+      <c r="Q19" s="21">
         <v>2386.8440000000001</v>
       </c>
-      <c r="R19" s="22">
+      <c r="R19" s="19">
+        <v>5601</v>
+      </c>
+      <c r="S19" s="19">
         <v>63090</v>
       </c>
-      <c r="S19" s="22">
-        <v>5601</v>
-      </c>
-      <c r="T19" s="23">
-        <v>0</v>
-      </c>
-      <c r="U19" s="22">
+      <c r="T19" s="20">
+        <v>0</v>
+      </c>
+      <c r="U19" s="19">
         <f t="shared" si="1"/>
         <v>201710.19500000001</v>
       </c>
-      <c r="V19" s="22">
+      <c r="V19" s="19">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -2412,73 +2412,73 @@
         <v>65</v>
       </c>
     </row>
-    <row r="20" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A20" s="27" t="s">
+    <row r="20" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A20" s="24" t="s">
         <v>81</v>
       </c>
-      <c r="B20" s="23">
+      <c r="B20" s="20">
         <v>262458.24099999998</v>
       </c>
-      <c r="C20" s="22">
+      <c r="C20" s="19">
         <v>15931.112999999999</v>
       </c>
-      <c r="D20" s="23">
-        <v>0</v>
-      </c>
-      <c r="E20" s="23" t="s">
+      <c r="D20" s="20">
+        <v>0</v>
+      </c>
+      <c r="E20" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="F20" s="23">
+      <c r="F20" s="20">
         <v>4132.2299999999996</v>
       </c>
-      <c r="G20" s="23">
-        <v>0</v>
-      </c>
-      <c r="H20" s="23">
+      <c r="G20" s="20">
+        <v>0</v>
+      </c>
+      <c r="H20" s="20">
         <v>368.24799999999999</v>
       </c>
-      <c r="I20" s="23">
-        <v>0</v>
-      </c>
-      <c r="J20" s="23">
-        <v>0</v>
-      </c>
-      <c r="K20" s="23">
-        <v>0</v>
-      </c>
-      <c r="L20" s="23">
+      <c r="I20" s="20">
+        <v>0</v>
+      </c>
+      <c r="J20" s="20">
+        <v>0</v>
+      </c>
+      <c r="K20" s="20">
+        <v>0</v>
+      </c>
+      <c r="L20" s="20">
         <v>2916.86</v>
       </c>
-      <c r="M20" s="23">
+      <c r="M20" s="20">
         <v>806.96</v>
       </c>
-      <c r="N20" s="23">
-        <v>0</v>
-      </c>
-      <c r="O20" s="22">
+      <c r="N20" s="20">
+        <v>0</v>
+      </c>
+      <c r="O20" s="19">
         <f t="shared" si="0"/>
         <v>40.161999999999352</v>
       </c>
-      <c r="P20" s="23">
+      <c r="P20" s="20">
         <v>94414.698000000004</v>
       </c>
-      <c r="Q20" s="24">
+      <c r="Q20" s="21">
         <v>42786</v>
       </c>
-      <c r="R20" s="23">
+      <c r="R20" s="20">
+        <v>17725</v>
+      </c>
+      <c r="S20" s="20">
         <v>87469.2</v>
       </c>
-      <c r="S20" s="23">
-        <v>17725</v>
-      </c>
-      <c r="T20" s="22">
-        <v>0</v>
-      </c>
-      <c r="U20" s="22">
+      <c r="T20" s="19">
+        <v>0</v>
+      </c>
+      <c r="U20" s="19">
         <f t="shared" si="1"/>
         <v>262458.24100000004</v>
       </c>
-      <c r="V20" s="22">
+      <c r="V20" s="19">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -2486,73 +2486,73 @@
         <v>65</v>
       </c>
     </row>
-    <row r="21" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A21" s="26" t="s">
+    <row r="21" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A21" s="23" t="s">
         <v>82</v>
       </c>
-      <c r="B21" s="22">
+      <c r="B21" s="19">
         <v>75463.909</v>
       </c>
-      <c r="C21" s="23">
+      <c r="C21" s="20">
         <v>42.006</v>
       </c>
-      <c r="D21" s="22">
-        <v>0</v>
-      </c>
-      <c r="E21" s="22" t="s">
+      <c r="D21" s="19">
+        <v>0</v>
+      </c>
+      <c r="E21" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="F21" s="22">
+      <c r="F21" s="19">
         <v>2732.73</v>
       </c>
-      <c r="G21" s="22">
-        <v>0</v>
-      </c>
-      <c r="H21" s="22">
+      <c r="G21" s="19">
+        <v>0</v>
+      </c>
+      <c r="H21" s="19">
         <v>46.030999999999999</v>
       </c>
-      <c r="I21" s="22">
-        <v>0</v>
-      </c>
-      <c r="J21" s="22">
-        <v>0</v>
-      </c>
-      <c r="K21" s="22">
-        <v>0</v>
-      </c>
-      <c r="L21" s="22">
+      <c r="I21" s="19">
+        <v>0</v>
+      </c>
+      <c r="J21" s="19">
+        <v>0</v>
+      </c>
+      <c r="K21" s="19">
+        <v>0</v>
+      </c>
+      <c r="L21" s="19">
         <v>1758.6949999999999</v>
       </c>
-      <c r="M21" s="22">
+      <c r="M21" s="19">
         <v>928.00400000000002</v>
       </c>
-      <c r="N21" s="22">
-        <v>0</v>
-      </c>
-      <c r="O21" s="22">
+      <c r="N21" s="19">
+        <v>0</v>
+      </c>
+      <c r="O21" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="P21" s="22">
+      <c r="P21" s="19">
         <v>6317.1729999999998</v>
       </c>
-      <c r="Q21" s="24">
+      <c r="Q21" s="21">
         <v>45952</v>
       </c>
-      <c r="R21" s="22">
+      <c r="R21" s="19">
+        <v>4184</v>
+      </c>
+      <c r="S21" s="19">
         <v>16236</v>
       </c>
-      <c r="S21" s="22">
-        <v>4184</v>
-      </c>
-      <c r="T21" s="23">
-        <v>0</v>
-      </c>
-      <c r="U21" s="22">
+      <c r="T21" s="20">
+        <v>0</v>
+      </c>
+      <c r="U21" s="19">
         <f t="shared" si="1"/>
         <v>75463.908999999985</v>
       </c>
-      <c r="V21" s="22">
+      <c r="V21" s="19">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -2560,73 +2560,73 @@
         <v>65</v>
       </c>
     </row>
-    <row r="22" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A22" s="27" t="s">
+    <row r="22" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A22" s="24" t="s">
         <v>83</v>
       </c>
-      <c r="B22" s="22">
+      <c r="B22" s="19">
         <v>24704.761999999999</v>
       </c>
-      <c r="C22" s="23">
+      <c r="C22" s="20">
         <v>426.83199999999999</v>
       </c>
-      <c r="D22" s="22">
-        <v>0</v>
-      </c>
-      <c r="E22" s="22" t="s">
+      <c r="D22" s="19">
+        <v>0</v>
+      </c>
+      <c r="E22" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="F22" s="22">
+      <c r="F22" s="19">
         <v>1781.8030000000001</v>
       </c>
-      <c r="G22" s="22">
-        <v>0</v>
-      </c>
-      <c r="H22" s="22">
+      <c r="G22" s="19">
+        <v>0</v>
+      </c>
+      <c r="H22" s="19">
         <v>46.030999999999999</v>
       </c>
-      <c r="I22" s="22">
-        <v>0</v>
-      </c>
-      <c r="J22" s="22">
-        <v>0</v>
-      </c>
-      <c r="K22" s="22">
-        <v>0</v>
-      </c>
-      <c r="L22" s="22">
+      <c r="I22" s="19">
+        <v>0</v>
+      </c>
+      <c r="J22" s="19">
+        <v>0</v>
+      </c>
+      <c r="K22" s="19">
+        <v>0</v>
+      </c>
+      <c r="L22" s="19">
         <v>1372.64</v>
       </c>
-      <c r="M22" s="22">
+      <c r="M22" s="19">
         <v>363.13200000000001</v>
       </c>
-      <c r="N22" s="22">
-        <v>0</v>
-      </c>
-      <c r="O22" s="22">
+      <c r="N22" s="19">
+        <v>0</v>
+      </c>
+      <c r="O22" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="P22" s="22">
+      <c r="P22" s="19">
         <v>10936.927</v>
       </c>
-      <c r="Q22" s="24">
+      <c r="Q22" s="21">
         <v>103</v>
       </c>
-      <c r="R22" s="22">
+      <c r="R22" s="19">
+        <v>2521</v>
+      </c>
+      <c r="S22" s="19">
         <v>8935.2000000000007</v>
       </c>
-      <c r="S22" s="22">
-        <v>2521</v>
-      </c>
-      <c r="T22" s="23">
-        <v>0</v>
-      </c>
-      <c r="U22" s="22">
+      <c r="T22" s="20">
+        <v>0</v>
+      </c>
+      <c r="U22" s="19">
         <f t="shared" si="1"/>
         <v>24704.761999999999</v>
       </c>
-      <c r="V22" s="22">
+      <c r="V22" s="19">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -2634,73 +2634,73 @@
         <v>65</v>
       </c>
     </row>
-    <row r="23" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A23" s="27" t="s">
+    <row r="23" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A23" s="24" t="s">
         <v>84</v>
       </c>
-      <c r="B23" s="23">
+      <c r="B23" s="20">
         <v>36138.853999999999</v>
       </c>
-      <c r="C23" s="22">
-        <v>0</v>
-      </c>
-      <c r="D23" s="23">
-        <v>0</v>
-      </c>
-      <c r="E23" s="23" t="s">
+      <c r="C23" s="19">
+        <v>0</v>
+      </c>
+      <c r="D23" s="20">
+        <v>0</v>
+      </c>
+      <c r="E23" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="F23" s="23">
-        <v>0</v>
-      </c>
-      <c r="G23" s="23">
-        <v>0</v>
-      </c>
-      <c r="H23" s="23">
-        <v>0</v>
-      </c>
-      <c r="I23" s="23">
-        <v>0</v>
-      </c>
-      <c r="J23" s="23">
-        <v>0</v>
-      </c>
-      <c r="K23" s="23">
-        <v>0</v>
-      </c>
-      <c r="L23" s="23">
-        <v>0</v>
-      </c>
-      <c r="M23" s="23">
-        <v>0</v>
-      </c>
-      <c r="N23" s="23">
-        <v>0</v>
-      </c>
-      <c r="O23" s="22">
+      <c r="F23" s="20">
+        <v>0</v>
+      </c>
+      <c r="G23" s="20">
+        <v>0</v>
+      </c>
+      <c r="H23" s="20">
+        <v>0</v>
+      </c>
+      <c r="I23" s="20">
+        <v>0</v>
+      </c>
+      <c r="J23" s="20">
+        <v>0</v>
+      </c>
+      <c r="K23" s="20">
+        <v>0</v>
+      </c>
+      <c r="L23" s="20">
+        <v>0</v>
+      </c>
+      <c r="M23" s="20">
+        <v>0</v>
+      </c>
+      <c r="N23" s="20">
+        <v>0</v>
+      </c>
+      <c r="O23" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="P23" s="23">
+      <c r="P23" s="20">
         <v>21828.853999999999</v>
       </c>
-      <c r="Q23" s="24">
-        <v>0</v>
-      </c>
-      <c r="R23" s="23">
+      <c r="Q23" s="21">
+        <v>0</v>
+      </c>
+      <c r="R23" s="20">
+        <v>0</v>
+      </c>
+      <c r="S23" s="20">
         <v>14310</v>
       </c>
-      <c r="S23" s="23">
-        <v>0</v>
-      </c>
-      <c r="T23" s="22">
-        <v>0</v>
-      </c>
-      <c r="U23" s="22">
+      <c r="T23" s="19">
+        <v>0</v>
+      </c>
+      <c r="U23" s="19">
         <f t="shared" si="1"/>
         <v>36138.853999999999</v>
       </c>
-      <c r="V23" s="22">
+      <c r="V23" s="19">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -2708,73 +2708,73 @@
         <v>65</v>
       </c>
     </row>
-    <row r="24" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A24" s="26" t="s">
+    <row r="24" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A24" s="23" t="s">
         <v>85</v>
       </c>
-      <c r="B24" s="23">
+      <c r="B24" s="20">
         <v>116123.69500000001</v>
       </c>
-      <c r="C24" s="22">
+      <c r="C24" s="19">
         <v>357.05099999999999</v>
       </c>
-      <c r="D24" s="23">
-        <v>0</v>
-      </c>
-      <c r="E24" s="23" t="s">
+      <c r="D24" s="20">
+        <v>0</v>
+      </c>
+      <c r="E24" s="20" t="s">
         <v>68</v>
       </c>
-      <c r="F24" s="23">
+      <c r="F24" s="20">
         <v>14725.132</v>
       </c>
-      <c r="G24" s="23">
+      <c r="G24" s="20">
         <v>2461.9839999999999</v>
       </c>
-      <c r="H24" s="23">
+      <c r="H24" s="20">
         <v>1565.0540000000001</v>
       </c>
-      <c r="I24" s="23">
-        <v>0</v>
-      </c>
-      <c r="J24" s="23">
-        <v>0</v>
-      </c>
-      <c r="K24" s="23">
-        <v>0</v>
-      </c>
-      <c r="L24" s="23">
+      <c r="I24" s="20">
+        <v>0</v>
+      </c>
+      <c r="J24" s="20">
+        <v>0</v>
+      </c>
+      <c r="K24" s="20">
+        <v>0</v>
+      </c>
+      <c r="L24" s="20">
         <v>10294.799999999999</v>
       </c>
-      <c r="M24" s="23">
+      <c r="M24" s="20">
         <v>363.13200000000001</v>
       </c>
-      <c r="N24" s="23">
-        <v>0</v>
-      </c>
-      <c r="O24" s="22">
+      <c r="N24" s="20">
+        <v>0</v>
+      </c>
+      <c r="O24" s="19">
         <f t="shared" si="0"/>
         <v>40.162000000000262</v>
       </c>
-      <c r="P24" s="23">
+      <c r="P24" s="20">
         <v>27508.82</v>
       </c>
-      <c r="Q24" s="24">
+      <c r="Q24" s="21">
         <v>4089.692</v>
       </c>
-      <c r="R24" s="23">
+      <c r="R24" s="20">
+        <v>6434</v>
+      </c>
+      <c r="S24" s="20">
         <v>63003.6</v>
       </c>
-      <c r="S24" s="23">
-        <v>6434</v>
-      </c>
-      <c r="T24" s="22">
+      <c r="T24" s="19">
         <v>5.4</v>
       </c>
-      <c r="U24" s="22">
+      <c r="U24" s="19">
         <f t="shared" si="1"/>
         <v>116123.69500000001</v>
       </c>
-      <c r="V24" s="22">
+      <c r="V24" s="19">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -2782,97 +2782,97 @@
         <v>65</v>
       </c>
     </row>
-    <row r="25" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A25" s="21"/>
-      <c r="B25" s="24"/>
-      <c r="C25" s="24"/>
-      <c r="D25" s="24"/>
-      <c r="E25" s="24"/>
-      <c r="F25" s="24"/>
-      <c r="G25" s="24"/>
-      <c r="H25" s="24"/>
-      <c r="I25" s="24"/>
-      <c r="J25" s="24"/>
-      <c r="K25" s="24"/>
-      <c r="L25" s="24"/>
-      <c r="M25" s="24"/>
-      <c r="N25" s="24"/>
-      <c r="O25" s="22"/>
-      <c r="P25" s="24"/>
-      <c r="Q25" s="24"/>
-      <c r="R25" s="24"/>
-      <c r="S25" s="24"/>
-      <c r="T25" s="24"/>
-      <c r="U25" s="22"/>
-      <c r="V25" s="22"/>
-    </row>
-    <row r="26" spans="1:26" x14ac:dyDescent="0.3">
-      <c r="A26" s="26" t="s">
+    <row r="25" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A25" s="18"/>
+      <c r="B25" s="21"/>
+      <c r="C25" s="21"/>
+      <c r="D25" s="21"/>
+      <c r="E25" s="21"/>
+      <c r="F25" s="21"/>
+      <c r="G25" s="21"/>
+      <c r="H25" s="21"/>
+      <c r="I25" s="21"/>
+      <c r="J25" s="21"/>
+      <c r="K25" s="21"/>
+      <c r="L25" s="21"/>
+      <c r="M25" s="21"/>
+      <c r="N25" s="21"/>
+      <c r="O25" s="19"/>
+      <c r="P25" s="21"/>
+      <c r="Q25" s="21"/>
+      <c r="R25" s="21"/>
+      <c r="S25" s="21"/>
+      <c r="T25" s="21"/>
+      <c r="U25" s="19"/>
+      <c r="V25" s="19"/>
+    </row>
+    <row r="26" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A26" s="23" t="s">
         <v>86</v>
       </c>
-      <c r="B26" s="22">
+      <c r="B26" s="19">
         <v>53893.033000000003</v>
       </c>
-      <c r="C26" s="23">
-        <v>0</v>
-      </c>
-      <c r="D26" s="22">
-        <v>0</v>
-      </c>
-      <c r="E26" s="22" t="s">
+      <c r="C26" s="20">
+        <v>0</v>
+      </c>
+      <c r="D26" s="19">
+        <v>0</v>
+      </c>
+      <c r="E26" s="19" t="s">
         <v>68</v>
       </c>
-      <c r="F26" s="22">
-        <v>0</v>
-      </c>
-      <c r="G26" s="22">
-        <v>0</v>
-      </c>
-      <c r="H26" s="22">
-        <v>0</v>
-      </c>
-      <c r="I26" s="22">
-        <v>0</v>
-      </c>
-      <c r="J26" s="22">
-        <v>0</v>
-      </c>
-      <c r="K26" s="22">
-        <v>0</v>
-      </c>
-      <c r="L26" s="22">
-        <v>0</v>
-      </c>
-      <c r="M26" s="22">
-        <v>0</v>
-      </c>
-      <c r="N26" s="22">
-        <v>0</v>
-      </c>
-      <c r="O26" s="22">
+      <c r="F26" s="19">
+        <v>0</v>
+      </c>
+      <c r="G26" s="19">
+        <v>0</v>
+      </c>
+      <c r="H26" s="19">
+        <v>0</v>
+      </c>
+      <c r="I26" s="19">
+        <v>0</v>
+      </c>
+      <c r="J26" s="19">
+        <v>0</v>
+      </c>
+      <c r="K26" s="19">
+        <v>0</v>
+      </c>
+      <c r="L26" s="19">
+        <v>0</v>
+      </c>
+      <c r="M26" s="19">
+        <v>0</v>
+      </c>
+      <c r="N26" s="19">
+        <v>0</v>
+      </c>
+      <c r="O26" s="19">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="P26" s="22">
+      <c r="P26" s="19">
         <v>13816.061</v>
       </c>
-      <c r="Q26" s="24">
+      <c r="Q26" s="21">
         <v>18923.371999999999</v>
       </c>
-      <c r="R26" s="22">
+      <c r="R26" s="19">
+        <v>0</v>
+      </c>
+      <c r="S26" s="19">
         <v>21153.599999999999</v>
       </c>
-      <c r="S26" s="22">
-        <v>0</v>
-      </c>
-      <c r="T26" s="23">
-        <v>0</v>
-      </c>
-      <c r="U26" s="22">
+      <c r="T26" s="20">
+        <v>0</v>
+      </c>
+      <c r="U26" s="19">
         <f t="shared" si="1"/>
         <v>53893.032999999996</v>
       </c>
-      <c r="V26" s="22">
+      <c r="V26" s="19">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
@@ -2880,23 +2880,23 @@
         <v>65</v>
       </c>
     </row>
-    <row r="28" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A28" s="1" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="29" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A29" s="1" t="s">
         <v>68</v>
       </c>
       <c r="S29" s="15"/>
     </row>
-    <row r="30" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A30" s="1" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="31" spans="1:26" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:26" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A31" s="1" t="s">
         <v>69</v>
       </c>

</xml_diff>